<commit_message>
adding more student feedback
</commit_message>
<xml_diff>
--- a/needed.xlsx
+++ b/needed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>jobs</t>
   </si>
@@ -28,28 +28,19 @@
     <t>Teaches Python/Scripting languages</t>
   </si>
   <si>
+    <t>Engineering as a core focus</t>
+  </si>
+  <si>
     <t>Teaches SQL/database languages</t>
   </si>
   <si>
+    <t>Traditional Machine Learning math/statistics</t>
+  </si>
+  <si>
+    <t>Business Problem Solving</t>
+  </si>
+  <si>
     <t>Teaches Big data technologies</t>
-  </si>
-  <si>
-    <t>Engineering</t>
-  </si>
-  <si>
-    <t>Engineering as a core focus</t>
-  </si>
-  <si>
-    <t>Traditional Machine Learning math/statistics</t>
-  </si>
-  <si>
-    <t>Modern Machine Learning math/research</t>
-  </si>
-  <si>
-    <t>Business Problem Solving</t>
-  </si>
-  <si>
-    <t>Problem solving using machine learning</t>
   </si>
   <si>
     <t>Business Communication/ interaction</t>
@@ -425,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -461,13 +452,13 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>0.33</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>0.38</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>-0.04</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -475,13 +466,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C4">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D4">
-        <v>-0.42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -489,13 +480,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>0.38</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0.29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -503,13 +494,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C6">
+        <v>0.62</v>
+      </c>
+      <c r="D6">
         <v>0.38</v>
-      </c>
-      <c r="D6">
-        <v>-0.04</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -517,13 +508,13 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>-0.42</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -531,59 +522,17 @@
         <v>9</v>
       </c>
       <c r="B8">
+        <v>0.83</v>
+      </c>
+      <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8">
         <v>0.33</v>
       </c>
-      <c r="C8">
-        <v>0.62</v>
-      </c>
-      <c r="D8">
-        <v>-0.29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>0.62</v>
-      </c>
-      <c r="D9">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>0.67</v>
-      </c>
-      <c r="C10">
-        <v>0.5</v>
-      </c>
-      <c r="D10">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>0.83</v>
-      </c>
-      <c r="C11">
-        <v>0.5</v>
-      </c>
-      <c r="D11">
-        <v>0.33</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>

</xml_diff>